<commit_message>
Top Deals - Second Commit
Manual Testing
</commit_message>
<xml_diff>
--- a/BestBuy - Top Deals.xlsx
+++ b/BestBuy - Top Deals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karriv\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AA42E2-BDA3-4887-B309-F9F999C1DA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA0C827-DF85-4710-914E-B6B8E601FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{DD388810-6835-4DCF-BF58-5291B40C8013}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{DD388810-6835-4DCF-BF58-5291B40C8013}"/>
   </bookViews>
   <sheets>
     <sheet name="User Story" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="199">
   <si>
     <t>Issue Type</t>
   </si>
@@ -232,9 +232,6 @@
     <t>As a user, I want to refresh my page, so that I can view if saved items remain</t>
   </si>
   <si>
-    <t xml:space="preserve">1. To validate Top Deals Functionality  by clicking on “Computers &amp; Tablets”                                                                                       2. Click "Laptops"                                                       3. Validate laptop deals are displayed                                                          </t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Checkbox first item                                                              2. Checkbox second item                                                         3. Click “Compare”                                                                4. Validate comparison table                                          5. Toggle ON in "All Specs"                                                                                                           6. Remove items                                              </t>
   </si>
   <si>
@@ -244,9 +241,6 @@
     <t xml:space="preserve">Click "Laptops"          </t>
   </si>
   <si>
-    <t xml:space="preserve">To validate Top Deals Functionality  by clicking on “Computers &amp; Tablets”                                                                                                                                       </t>
-  </si>
-  <si>
     <t xml:space="preserve">Save first laptop                                                                    </t>
   </si>
   <si>
@@ -277,15 +271,6 @@
     <t>Refresh page and validate saved items remain</t>
   </si>
   <si>
-    <t>Pop-up appears</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Save first laptop                                                                2. Save second laptop                                                         3. Validate Pop-up for add &amp; remove                                                        4. Click "See all your saved items"                                                5.Validate saved items list                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate Pop-up for add &amp; remove                                                              </t>
-  </si>
-  <si>
     <t>Scroll through laptop deals</t>
   </si>
   <si>
@@ -307,9 +292,6 @@
     <t>1. Review  the first laptop                                       2. Click “Save” on first laptop    3. Check if Pop-up appears</t>
   </si>
   <si>
-    <t>1. Check if Pop-up appears while item is added                               2. Check if Pop-up appears while item is removed</t>
-  </si>
-  <si>
     <t>1. Scroll up                                         2. Click “Saved Items”</t>
   </si>
   <si>
@@ -388,12 +370,6 @@
     <t>Second laptop is saved</t>
   </si>
   <si>
-    <t>Pop-up should appear when item is added or removed</t>
-  </si>
-  <si>
-    <t>Pop-up appears when item is added or removed</t>
-  </si>
-  <si>
     <t>Saved Items page should be opened</t>
   </si>
   <si>
@@ -604,8 +580,65 @@
     <t xml:space="preserve">Top Deals </t>
   </si>
   <si>
-    <t>1. Open Best Buy homepage in  browser
-2. Navigate to "Top Deals"                          3. Click “Computers &amp; Tablets”</t>
+    <t xml:space="preserve">To validate Top Deals Functionality  by clicking on “Top Deals”                                                                                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Computers &amp; Tablets"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Best Buy homepage in  browser
+2. Navigate to "Top Deals"                          </t>
+  </si>
+  <si>
+    <t>1. Check if options for "Top Deals" are there                                          3. Click “Computers &amp; Tablets”</t>
+  </si>
+  <si>
+    <t>Top Deals should appear</t>
+  </si>
+  <si>
+    <t>Top Deals appeared</t>
+  </si>
+  <si>
+    <t>All Electronics Deals are displayed</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_05</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_06</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_07</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_08</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_09</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_10</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_11</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_12</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_13</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_14</t>
+  </si>
+  <si>
+    <t>TS_BestBuy_TopDeals_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. To validate Top Deals Functionality  by clicking on “Top Deals”                                                                                2. Click "Computers &amp; Tablets"                                                          3. Click "Laptops"                                                                4. Validate laptop deals are displayed                                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Save first laptop                                                                2. Save second laptop                                                                                                               3. Click "See all your saved items"                                                4.Validate saved items list                        </t>
   </si>
 </sst>
 </file>
@@ -808,7 +841,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -819,22 +852,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -865,17 +891,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -1229,47 +1277,47 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="62.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.90625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="94.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.90625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:3" s="20" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1280,7 +1328,7 @@
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1291,18 +1339,18 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:3" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="21" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1313,18 +1361,18 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="21" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1335,7 +1383,7 @@
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="22" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1346,7 +1394,7 @@
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="22" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1357,7 +1405,7 @@
       <c r="B11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="22" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1368,18 +1416,18 @@
       <c r="B12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="21" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1397,8 +1445,8 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A2" zoomScale="98" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1408,26 +1456,26 @@
     <col min="3" max="3" width="28.453125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.81640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.36328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="34.81640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="23" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1445,13 +1493,13 @@
         <v>21</v>
       </c>
       <c r="E2" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1465,13 +1513,13 @@
         <v>21</v>
       </c>
       <c r="E3" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="93.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="104.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1488,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.35">
@@ -1508,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1524,8 +1572,8 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView zoomScale="96" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1541,38 +1589,38 @@
     <col min="9" max="9" width="13.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9" s="24" customFormat="1" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
@@ -1581,428 +1629,428 @@
         <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>67</v>
+        <v>179</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" t="s">
-        <v>115</v>
-      </c>
-      <c r="H7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>105</v>
+      <c r="I8" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H9" t="s">
-        <v>120</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>105</v>
+      <c r="D9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>105</v>
+        <v>115</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>105</v>
+        <v>116</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>192</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>105</v>
+        <v>118</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>47</v>
+        <v>193</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>105</v>
+        <v>120</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>194</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>135</v>
+        <v>122</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>195</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" t="s">
-        <v>134</v>
-      </c>
-      <c r="H16" t="s">
-        <v>133</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>105</v>
+      <c r="D16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17" ht="39" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2019,8 +2067,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2034,43 +2082,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="A1" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>143</v>
+      <c r="E2" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2088,8 +2136,8 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="81" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2098,229 +2146,229 @@
     <col min="2" max="2" width="23.453125" customWidth="1"/>
     <col min="3" max="3" width="22.90625" customWidth="1"/>
     <col min="4" max="4" width="23.7265625" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
     <col min="6" max="6" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>150</v>
+    <row r="1" spans="1:6" s="16" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>105</v>
+        <v>144</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D3" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>105</v>
+        <v>145</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>105</v>
+        <v>146</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D6" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>105</v>
+        <v>148</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D7" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>105</v>
+        <v>149</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D8" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>105</v>
+        <v>150</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D9" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>105</v>
+        <v>151</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>105</v>
+        <v>152</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D11" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>105</v>
+        <v>153</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D12" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>105</v>
+        <v>154</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D13" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>105</v>
+        <v>155</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D14" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>135</v>
+        <v>156</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>127</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D15" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>105</v>
+        <v>157</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>105</v>
+        <v>158</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2337,7 +2385,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2354,73 +2402,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" s="26" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-    </row>
-    <row r="2" spans="1:9" s="24" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="23" t="s">
+      <c r="I2" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="23" t="s">
+    </row>
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="B3" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="15" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" s="21">
+      <c r="C3" s="17">
         <v>15</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="17">
         <v>14</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="17">
         <v>1</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="17">
         <v>15</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="18">
         <v>0.93330000000000002</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="18">
         <v>6.6600000000000006E-2</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="18">
         <v>1</v>
       </c>
     </row>

</xml_diff>